<commit_message>
Updated experiment results spreadsheet
</commit_message>
<xml_diff>
--- a/docs/Experiment 1 - Usokin/Experiment 1C Results.xlsx
+++ b/docs/Experiment 1 - Usokin/Experiment 1C Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="820" windowWidth="31320" windowHeight="17720" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="1560" windowWidth="27760" windowHeight="16080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VAE - Model Selection Results" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="1372">
   <si>
     <t>model_name</t>
   </si>
@@ -4104,13 +4104,46 @@
   </si>
   <si>
     <t>adam:lr=0.0005912082623654395</t>
+  </si>
+  <si>
+    <t>Model Type</t>
+  </si>
+  <si>
+    <t>Optimal K</t>
+  </si>
+  <si>
+    <t>PAC (Opt. K)</t>
+  </si>
+  <si>
+    <t>Force K</t>
+  </si>
+  <si>
+    <t>PAC (Force K)</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Adjusted Rand Index (ARI)</t>
+  </si>
+  <si>
+    <t># Genes</t>
+  </si>
+  <si>
+    <t># Encoder Layers</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>VAE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4122,6 +4155,13 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4165,12 +4205,23 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF53B367"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4191,22 +4242,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -4215,16 +4275,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4556,7 +4628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="AO1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -20884,15 +20956,559 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1364</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1365</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D2" s="10">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.13507412099999999</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.13507412099999999</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.91494727899999995</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.95498392300000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2">
+        <v>100</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9.6053974E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4">
+        <v>9.6053974E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.91358476899999996</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.95337620599999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D4" s="10">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.129979133334369</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.129979133334369</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.88931827892455995</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.93890675241157595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2">
+        <v>500</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.1098430000000002E-3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4">
+        <v>7.5865604000000003E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.88512236300000002</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.937299035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2">
+        <v>500</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.6108237000000001E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4">
+        <v>8.3989623999999999E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.88949989299999999</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.93569131800000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7.2106497662208599E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.23026857418022001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.85109540921461202</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.92604501607717005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2">
+        <v>500</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3.5333530000000002E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3.5333530000000002E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.86435917200000001</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.92443729900000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2">
+        <v>100</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.15812065385670901</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.18788801383516901</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.84440838597077394</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.91961414790996798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2">
+        <v>500</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.102308795584344</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.102308795584344</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.83225341949668796</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.91318327974276503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5.7272007E-2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5.7272007E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.84326704500000005</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.91157556299999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2">
+        <v>500</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.109676851463514</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.144471886957557</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.83694743048408604</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.91157556270096496</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2">
+        <v>500</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.16325188602554699</v>
+      </c>
+      <c r="F13" s="2">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.184988427543999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.83515199405339902</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.90353697749196105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.0070885E-2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.13898856200000001</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.79132191399999996</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.88102893900000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D15" s="10">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6.0477085999999999E-2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4</v>
+      </c>
+      <c r="G15" s="4">
+        <v>6.0477085999999999E-2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.72146050799999994</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0.852090032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D16" s="2">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.16006234110525999</v>
+      </c>
+      <c r="F16" s="2">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.18744272022616801</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.70506883146312604</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.842443729903537</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D17" s="2">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.15964811449223601</v>
+      </c>
+      <c r="F17" s="2">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.31839528610114398</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.51696761058560703</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.76848874598070704</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:H17">
+    <sortCondition descending="1" ref="G1"/>
+  </sortState>
+  <conditionalFormatting sqref="H2:H17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF54B468"/>
+        <color rgb="FFFFEB84"/>
+        <color theme="5"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>